<commit_message>
bug fix date format in excel
</commit_message>
<xml_diff>
--- a/public/imports/clients.xlsx
+++ b/public/imports/clients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Alraqiah\public\imports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\promo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -60,6 +60,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,14 +94,14 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -114,8 +117,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J1048575" totalsRowShown="0">
-  <autoFilter ref="A1:J1048575"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J1048572" totalsRowShown="0">
+  <autoFilter ref="A1:J1048572"/>
   <tableColumns count="10">
     <tableColumn id="1" name="name"/>
     <tableColumn id="2" name="phone"/>
@@ -398,11 +401,13 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>

</xml_diff>